<commit_message>
Added percentage comparison graph.
</commit_message>
<xml_diff>
--- a/Final Tables and graphs/year_movies_moviesWithAAActors_edited.xlsx
+++ b/Final Tables and graphs/year_movies_moviesWithAAActors_edited.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC8DB67-0D0C-4A90-A957-0920C9D00343}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F29CC-C86E-4A15-B9B5-2B395CFF9FDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>year</t>
   </si>
@@ -29,6 +35,9 @@
   </si>
   <si>
     <t>num_of_movies_with_AAActors</t>
+  </si>
+  <si>
+    <t>percentage</t>
   </si>
 </sst>
 </file>
@@ -72,6 +81,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF652B91"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1343,7 +1357,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1376,7 +1390,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -2637,6 +2651,1048 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="he-IL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>% of movies with African-American actors</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="652B91"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>גיליון1!$A$2:$A$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="107"/>
+                <c:pt idx="0">
+                  <c:v>1912</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1913</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1914</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1915</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1916</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1917</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1918</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1919</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1921</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1922</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1923</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1924</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1925</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1926</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1927</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1928</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1929</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1930</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1931</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1932</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1933</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1934</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1935</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1936</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1937</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1938</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1939</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1942</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1945</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1946</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1947</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1948</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1949</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1951</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1955</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1956</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1957</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1958</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1959</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1960</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1961</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1962</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1963</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1964</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1966</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1967</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1969</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$D$2:$D$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="107"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0909090909090917</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8461538461538463</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.3255813953488373</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.92592592592592582</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.9411764705882351</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.1914893617021276</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.8018018018018018</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.3057851239669422</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.6528925619834711</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.7699115044247788</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.7272727272727271</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.669724770642202</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.1546391752577314</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.8018018018018018</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.4793388429752068</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.5423728813559325</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.4598540145985401</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.75187969924812026</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.79365079365079361</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.74074074074074081</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.7777777777777777</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.80645161290322576</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4814814814814816</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.0979020979020979</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.4347826086956523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.0408163265306123</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.197802197802198</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.197802197802198</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.9411764705882351</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.7037037037037033</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.8691588785046727</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.8037383177570092</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.1282051282051277</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.9019607843137258</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.9099099099099099</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7.6335877862595423</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>16.788321167883211</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>17.293233082706767</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>14.40677966101695</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>20.754716981132077</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>10.569105691056912</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.7586206896551726</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.0175438596491224</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.5555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>8.2191780821917799</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.6176470588235299</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9.2198581560283674</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>10.606060606060606</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>10.857142857142858</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.0459770114942533</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>14.606741573033707</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>10.232558139534884</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>11.864406779661017</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10.859728506787331</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9.8654708520179373</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>11.312217194570136</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>16.826923076923077</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>14.468085106382977</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>13.865546218487395</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>15.107913669064748</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>17.562724014336915</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>18.14946619217082</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>13.768115942028986</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>18.560606060606062</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>16.117216117216117</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>16.891891891891891</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>16.030534351145036</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>17.79935275080906</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>15.405405405405407</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>15.776699029126215</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>13.140311804008908</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>12.153518123667377</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>12.114989733059549</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10.779816513761469</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.1262135922330092</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>9.2198581560283674</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>11.475409836065573</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>9.9573257467994303</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>8.9481946624803772</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>11.208406304728546</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>18.085106382978726</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DE7B-480B-9B13-E8B6C1C7D4AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="456292208"/>
+        <c:axId val="456289912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="456292208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="1"/>
+                  <a:t>YEAR</a:t>
+                </a:r>
+                <a:endParaRPr lang="he-IL" sz="1100" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="he-IL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="3600000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="he-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456289912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="456289912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:endParaRPr lang="he-IL" sz="1100" b="1" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="he-IL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:headEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="he-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456292208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="he-IL"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="he-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="he-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2717,6 +3773,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="293">
   <cs:axisTitle>
@@ -3271,6 +4367,559 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="293">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="75000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="51000">
+            <a:schemeClr val="phClr">
+              <a:alpha val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+              <a:alpha val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="75000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="51000">
+            <a:schemeClr val="phClr">
+              <a:alpha val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+              <a:alpha val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:headEnd type="none" w="sm" len="sm"/>
+        <a:tailEnd type="none" w="sm" len="sm"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="293">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3894,6 +5543,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>128589</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="תרשים 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C70F74-1CB9-4BD4-A249-708DF8C9A155}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4165,15 +5852,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="P5" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.25" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4183,8 +5874,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1912</v>
       </c>
@@ -4194,8 +5888,12 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>100*(C2/B2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1913</v>
       </c>
@@ -4205,8 +5903,11 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1914</v>
       </c>
@@ -4216,8 +5917,12 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" ref="D4:D67" si="0">100*(C4/B4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1915</v>
       </c>
@@ -4227,8 +5932,12 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1916</v>
       </c>
@@ -4238,8 +5947,12 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1917</v>
       </c>
@@ -4249,8 +5962,12 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1918</v>
       </c>
@@ -4260,8 +5977,12 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1919</v>
       </c>
@@ -4271,8 +5992,12 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1920</v>
       </c>
@@ -4282,8 +6007,12 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1921</v>
       </c>
@@ -4293,8 +6022,12 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1922</v>
       </c>
@@ -4304,8 +6037,12 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1923</v>
       </c>
@@ -4315,8 +6052,12 @@
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1924</v>
       </c>
@@ -4326,8 +6067,12 @@
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1925</v>
       </c>
@@ -4337,8 +6082,12 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>3.8461538461538463</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1926</v>
       </c>
@@ -4348,8 +6097,12 @@
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1927</v>
       </c>
@@ -4359,8 +6112,12 @@
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1928</v>
       </c>
@@ -4370,8 +6127,12 @@
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1929</v>
       </c>
@@ -4381,8 +6142,12 @@
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>2.3255813953488373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1930</v>
       </c>
@@ -4392,8 +6157,12 @@
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1931</v>
       </c>
@@ -4403,8 +6172,12 @@
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1932</v>
       </c>
@@ -4414,8 +6187,12 @@
       <c r="C22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1933</v>
       </c>
@@ -4425,8 +6202,12 @@
       <c r="C23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.92592592592592582</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1934</v>
       </c>
@@ -4436,8 +6217,12 @@
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1935</v>
       </c>
@@ -4447,8 +6232,12 @@
       <c r="C25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1936</v>
       </c>
@@ -4458,8 +6247,12 @@
       <c r="C26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2.9411764705882351</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1937</v>
       </c>
@@ -4469,8 +6262,12 @@
       <c r="C27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1938</v>
       </c>
@@ -4480,8 +6277,12 @@
       <c r="C28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>3.1914893617021276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1939</v>
       </c>
@@ -4491,8 +6292,12 @@
       <c r="C29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>1.8018018018018018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1940</v>
       </c>
@@ -4502,8 +6307,12 @@
       <c r="C30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1941</v>
       </c>
@@ -4513,8 +6322,12 @@
       <c r="C31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3.3057851239669422</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1942</v>
       </c>
@@ -4524,8 +6337,12 @@
       <c r="C32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1.6528925619834711</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1943</v>
       </c>
@@ -4535,8 +6352,12 @@
       <c r="C33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1.7699115044247788</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1944</v>
       </c>
@@ -4546,8 +6367,12 @@
       <c r="C34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>2.7272727272727271</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1945</v>
       </c>
@@ -4557,8 +6382,12 @@
       <c r="C35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>3.669724770642202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1946</v>
       </c>
@@ -4568,8 +6397,12 @@
       <c r="C36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>5.1546391752577314</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1947</v>
       </c>
@@ -4579,8 +6412,12 @@
       <c r="C37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>1.8018018018018018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1948</v>
       </c>
@@ -4590,8 +6427,12 @@
       <c r="C38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>2.4793388429752068</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1949</v>
       </c>
@@ -4601,8 +6442,12 @@
       <c r="C39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>2.5423728813559325</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1950</v>
       </c>
@@ -4612,8 +6457,12 @@
       <c r="C40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>1.4598540145985401</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1951</v>
       </c>
@@ -4623,8 +6472,12 @@
       <c r="C41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1952</v>
       </c>
@@ -4634,8 +6487,12 @@
       <c r="C42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>0.79365079365079361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1953</v>
       </c>
@@ -4645,8 +6502,12 @@
       <c r="C43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>0.74074074074074081</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1954</v>
       </c>
@@ -4656,8 +6517,12 @@
       <c r="C44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777777</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1955</v>
       </c>
@@ -4667,8 +6532,12 @@
       <c r="C45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>0.80645161290322576</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1956</v>
       </c>
@@ -4678,8 +6547,12 @@
       <c r="C46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>1.4814814814814816</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1957</v>
       </c>
@@ -4689,8 +6562,12 @@
       <c r="C47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>2.0979020979020979</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1958</v>
       </c>
@@ -4700,8 +6577,12 @@
       <c r="C48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1959</v>
       </c>
@@ -4711,8 +6592,12 @@
       <c r="C49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1960</v>
       </c>
@@ -4722,8 +6607,12 @@
       <c r="C50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>5.4347826086956523</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1961</v>
       </c>
@@ -4733,8 +6622,12 @@
       <c r="C51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>2.0408163265306123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1962</v>
       </c>
@@ -4744,8 +6637,12 @@
       <c r="C52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>2.197802197802198</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1963</v>
       </c>
@@ -4755,8 +6652,12 @@
       <c r="C53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>2.197802197802198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1964</v>
       </c>
@@ -4766,8 +6667,12 @@
       <c r="C54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>2.9411764705882351</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1965</v>
       </c>
@@ -4777,8 +6682,12 @@
       <c r="C55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>3.7037037037037033</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1966</v>
       </c>
@@ -4788,8 +6697,12 @@
       <c r="C56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>1.8691588785046727</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1967</v>
       </c>
@@ -4799,8 +6712,12 @@
       <c r="C57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>2.8037383177570092</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1968</v>
       </c>
@@ -4810,8 +6727,12 @@
       <c r="C58">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>5.1282051282051277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1969</v>
       </c>
@@ -4821,8 +6742,12 @@
       <c r="C59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>4.9019607843137258</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1970</v>
       </c>
@@ -4832,8 +6757,12 @@
       <c r="C60">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>9.9099099099099099</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1971</v>
       </c>
@@ -4843,8 +6772,12 @@
       <c r="C61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>7.6335877862595423</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1972</v>
       </c>
@@ -4854,8 +6787,12 @@
       <c r="C62">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>16.788321167883211</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1973</v>
       </c>
@@ -4865,8 +6802,12 @@
       <c r="C63">
         <v>23</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>17.293233082706767</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1974</v>
       </c>
@@ -4876,8 +6817,12 @@
       <c r="C64">
         <v>17</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>14.40677966101695</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1975</v>
       </c>
@@ -4887,8 +6832,12 @@
       <c r="C65">
         <v>22</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>20.754716981132077</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1976</v>
       </c>
@@ -4898,8 +6847,12 @@
       <c r="C66">
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>10.569105691056912</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1977</v>
       </c>
@@ -4909,8 +6862,12 @@
       <c r="C67">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <f t="shared" si="0"/>
+        <v>7.7586206896551726</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1978</v>
       </c>
@@ -4920,8 +6877,12 @@
       <c r="C68">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <f t="shared" ref="D68:D108" si="1">100*(C68/B68)</f>
+        <v>7.0175438596491224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1979</v>
       </c>
@@ -4931,8 +6892,12 @@
       <c r="C69">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555554</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1980</v>
       </c>
@@ -4942,8 +6907,12 @@
       <c r="C70">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>8.2191780821917799</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1981</v>
       </c>
@@ -4953,8 +6922,12 @@
       <c r="C71">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>6.6176470588235299</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1982</v>
       </c>
@@ -4964,8 +6937,12 @@
       <c r="C72">
         <v>13</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>9.2198581560283674</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1983</v>
       </c>
@@ -4975,8 +6952,12 @@
       <c r="C73">
         <v>14</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>10.606060606060606</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1984</v>
       </c>
@@ -4986,8 +6967,12 @@
       <c r="C74">
         <v>19</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>10.857142857142858</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1985</v>
       </c>
@@ -4997,8 +6982,12 @@
       <c r="C75">
         <v>14</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>8.0459770114942533</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1986</v>
       </c>
@@ -5008,8 +6997,12 @@
       <c r="C76">
         <v>26</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>14.606741573033707</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1987</v>
       </c>
@@ -5019,8 +7012,12 @@
       <c r="C77">
         <v>22</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>10.232558139534884</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1988</v>
       </c>
@@ -5030,8 +7027,12 @@
       <c r="C78">
         <v>28</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>11.864406779661017</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1989</v>
       </c>
@@ -5041,8 +7042,12 @@
       <c r="C79">
         <v>24</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>10.859728506787331</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1990</v>
       </c>
@@ -5052,8 +7057,12 @@
       <c r="C80">
         <v>22</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>9.8654708520179373</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1991</v>
       </c>
@@ -5063,8 +7072,12 @@
       <c r="C81">
         <v>25</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>11.312217194570136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1992</v>
       </c>
@@ -5074,8 +7087,12 @@
       <c r="C82">
         <v>35</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>16.826923076923077</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1993</v>
       </c>
@@ -5085,8 +7102,12 @@
       <c r="C83">
         <v>34</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>14.468085106382977</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1994</v>
       </c>
@@ -5096,8 +7117,12 @@
       <c r="C84">
         <v>33</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>13.865546218487395</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1995</v>
       </c>
@@ -5107,8 +7132,12 @@
       <c r="C85">
         <v>42</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>15.107913669064748</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1996</v>
       </c>
@@ -5118,8 +7147,12 @@
       <c r="C86">
         <v>49</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>17.562724014336915</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1997</v>
       </c>
@@ -5129,8 +7162,12 @@
       <c r="C87">
         <v>51</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>18.14946619217082</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1998</v>
       </c>
@@ -5140,8 +7177,12 @@
       <c r="C88">
         <v>38</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>13.768115942028986</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1999</v>
       </c>
@@ -5151,8 +7192,12 @@
       <c r="C89">
         <v>49</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>18.560606060606062</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2000</v>
       </c>
@@ -5162,8 +7207,12 @@
       <c r="C90">
         <v>44</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>16.117216117216117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2001</v>
       </c>
@@ -5173,8 +7222,12 @@
       <c r="C91">
         <v>45</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2002</v>
       </c>
@@ -5184,8 +7237,12 @@
       <c r="C92">
         <v>50</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>16.891891891891891</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2003</v>
       </c>
@@ -5195,8 +7252,12 @@
       <c r="C93">
         <v>42</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>16.030534351145036</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2004</v>
       </c>
@@ -5206,8 +7267,12 @@
       <c r="C94">
         <v>55</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>17.79935275080906</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2005</v>
       </c>
@@ -5217,8 +7282,12 @@
       <c r="C95">
         <v>57</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>15.405405405405407</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2006</v>
       </c>
@@ -5228,8 +7297,12 @@
       <c r="C96">
         <v>65</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>15.776699029126215</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2007</v>
       </c>
@@ -5239,8 +7312,12 @@
       <c r="C97">
         <v>59</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>13.140311804008908</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2008</v>
       </c>
@@ -5250,8 +7327,12 @@
       <c r="C98">
         <v>57</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>12.153518123667377</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2009</v>
       </c>
@@ -5261,8 +7342,12 @@
       <c r="C99">
         <v>59</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>12.114989733059549</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2010</v>
       </c>
@@ -5272,8 +7357,12 @@
       <c r="C100">
         <v>47</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>10.779816513761469</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2011</v>
       </c>
@@ -5283,8 +7372,12 @@
       <c r="C101">
         <v>47</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>9.1262135922330092</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2012</v>
       </c>
@@ -5294,8 +7387,12 @@
       <c r="C102">
         <v>52</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102">
+        <f t="shared" si="1"/>
+        <v>9.2198581560283674</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2013</v>
       </c>
@@ -5305,8 +7402,12 @@
       <c r="C103">
         <v>70</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103">
+        <f t="shared" si="1"/>
+        <v>11.475409836065573</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -5316,8 +7417,12 @@
       <c r="C104">
         <v>70</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104">
+        <f t="shared" si="1"/>
+        <v>9.9573257467994303</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2015</v>
       </c>
@@ -5327,8 +7432,12 @@
       <c r="C105">
         <v>57</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <f t="shared" si="1"/>
+        <v>8.9481946624803772</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -5338,8 +7447,12 @@
       <c r="C106">
         <v>64</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>11.208406304728546</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2017</v>
       </c>
@@ -5349,8 +7462,12 @@
       <c r="C107">
         <v>34</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107">
+        <f t="shared" si="1"/>
+        <v>18.085106382978726</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2018</v>
       </c>
@@ -5358,6 +7475,10 @@
         <v>4</v>
       </c>
       <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>